<commit_message>
fixed issues with variables and setup file
</commit_message>
<xml_diff>
--- a/matlab/assets/timeDomainVariables.xlsx
+++ b/matlab/assets/timeDomainVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojok\Documents\repos\Studienarbeit\matlab\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D19AB0-05DB-4B5D-AD4C-8AE0FC6B6526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D793B87-9F57-469C-BA56-F72DBE437899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,12 +365,6 @@
     <t>Poincare_SD2_SD1</t>
   </si>
   <si>
-    <t>alpha 1</t>
-  </si>
-  <si>
-    <t>alpha 2</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -437,60 +431,33 @@
     <t>Recurrence plot analysis: Minimum line length</t>
   </si>
   <si>
-    <t>MSE01</t>
-  </si>
-  <si>
     <t>Multiscale entropy, MSE(1)</t>
   </si>
   <si>
     <t>Multiscale entropy for scale factor values τ = 1</t>
   </si>
   <si>
-    <t>MSE02</t>
-  </si>
-  <si>
     <t>Multiscale entropy for scale factor values τ = 2</t>
   </si>
   <si>
-    <t>MSE03</t>
-  </si>
-  <si>
     <t>Multiscale entropy for scale factor values τ = 3</t>
   </si>
   <si>
-    <t>MSE04</t>
-  </si>
-  <si>
     <t>Multiscale entropy for scale factor values τ = 4</t>
   </si>
   <si>
-    <t>MSE05</t>
-  </si>
-  <si>
     <t>Multiscale entropy for scale factor values τ = 5</t>
   </si>
   <si>
-    <t>MSE06</t>
-  </si>
-  <si>
     <t>Multiscale entropy for scale factor values τ = 6</t>
   </si>
   <si>
-    <t>MSE07</t>
-  </si>
-  <si>
     <t>Multiscale entropy for scale factor values τ = 7</t>
   </si>
   <si>
-    <t>MSE08</t>
-  </si>
-  <si>
     <t>Multiscale entropy for scale factor values τ = 8</t>
   </si>
   <si>
-    <t>MSE09</t>
-  </si>
-  <si>
     <t>Multiscale entropy for scale factor values τ = 9</t>
   </si>
   <si>
@@ -627,6 +594,39 @@
   </si>
   <si>
     <t>NonLinear</t>
+  </si>
+  <si>
+    <t>MSE1</t>
+  </si>
+  <si>
+    <t>MSE2</t>
+  </si>
+  <si>
+    <t>MSE3</t>
+  </si>
+  <si>
+    <t>MSE4</t>
+  </si>
+  <si>
+    <t>MSE5</t>
+  </si>
+  <si>
+    <t>MSE6</t>
+  </si>
+  <si>
+    <t>MSE8</t>
+  </si>
+  <si>
+    <t>MSE7</t>
+  </si>
+  <si>
+    <t>MSE9</t>
+  </si>
+  <si>
+    <t>alpha2</t>
+  </si>
+  <si>
+    <t>alpha1</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
         <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1131,7 +1131,7 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
         <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
         <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1216,7 +1216,7 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="E15" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1279,7 +1279,7 @@
         <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="C17" s="1"/>
       <c r="E17" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1333,7 +1333,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1367,7 +1367,7 @@
         <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
         <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1401,7 +1401,7 @@
         <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1418,7 +1418,7 @@
         <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
         <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1452,7 +1452,7 @@
         <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1469,7 +1469,7 @@
         <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1486,7 +1486,7 @@
         <v>78</v>
       </c>
       <c r="E10" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1503,7 +1503,7 @@
         <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1554,7 +1554,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1571,7 +1571,7 @@
         <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
         <v>79</v>
       </c>
       <c r="E16" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1604,7 +1604,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1629,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1640,13 +1640,13 @@
         <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1657,13 +1657,13 @@
         <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1674,13 +1674,13 @@
         <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1691,13 +1691,13 @@
         <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,506 +1708,506 @@
         <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
         <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>198</v>
       </c>
       <c r="B8" t="s">
         <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
         <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
         <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D10" t="s">
         <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
         <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
         <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
         <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D12" t="s">
         <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
         <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
         <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D14" t="s">
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
         <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C19" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="B22" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C22" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="B24" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C24" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C25" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D26" t="s">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B27" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C28" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C29" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C30" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B31" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C31" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D31" t="s">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B32" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C32" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D32" t="s">
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B33" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C33" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D33" t="s">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B34" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C34" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="D34" t="s">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C35" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D35" t="s">
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>